<commit_message>
can search patient by DOB now
blue theme, blue fab icon
all action icons on the left
moved symptoms to diagnosis
</commit_message>
<xml_diff>
--- a/docs/01-tcm-words-main.xlsx
+++ b/docs/01-tcm-words-main.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21380" yWindow="2120" windowWidth="15840" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="8300" yWindow="2180" windowWidth="15840" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="中医" sheetId="14" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>method of treatment </t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>herb</t>
+  </si>
+  <si>
+    <t>辩证</t>
+  </si>
+  <si>
+    <t>TCM syndrome differentiation</t>
   </si>
 </sst>
 </file>
@@ -406,20 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -428,53 +434,64 @@
     </row>
     <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>